<commit_message>
Update Power Budget SHEET, and Component Selection
</commit_message>
<xml_diff>
--- a/docs/Appendix/03-Power-Budget/DirksPowerBudget.xlsx
+++ b/docs/Appendix/03-Power-Budget/DirksPowerBudget.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Precision\Desktop\J2DIndivGithub\Classwork\JacobDirksEGR314.github.io\docs\Appendix\03-Power-Budget\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADE62186-5B36-4758-914A-5B85FA3FCB0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{857DAD5D-2939-4EF6-AFB0-F69557C7C322}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Power Budget" sheetId="1" r:id="rId1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="58">
   <si>
     <t>Team Number:</t>
   </si>
@@ -230,6 +230,12 @@
   </si>
   <si>
     <t>3.3V - 5V</t>
+  </si>
+  <si>
+    <t>RC Servo</t>
+  </si>
+  <si>
+    <t>3-9V</t>
   </si>
 </sst>
 </file>
@@ -608,15 +614,39 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -626,31 +656,7 @@
     <xf numFmtId="49" fontId="5" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1004,8 +1010,8 @@
   </sheetPr>
   <dimension ref="A1:H62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="D65" sqref="D65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1021,16 +1027,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="59" t="s">
         <v>44</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42"/>
+      <c r="B1" s="55"/>
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="55"/>
+      <c r="F1" s="55"/>
+      <c r="G1" s="55"/>
+      <c r="H1" s="55"/>
     </row>
     <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -1093,16 +1099,16 @@
       <c r="H6" s="5"/>
     </row>
     <row r="7" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="43" t="s">
+      <c r="A7" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="44"/>
-      <c r="C7" s="44"/>
-      <c r="D7" s="44"/>
-      <c r="E7" s="44"/>
-      <c r="F7" s="44"/>
-      <c r="G7" s="44"/>
-      <c r="H7" s="45"/>
+      <c r="B7" s="50"/>
+      <c r="C7" s="50"/>
+      <c r="D7" s="50"/>
+      <c r="E7" s="50"/>
+      <c r="F7" s="50"/>
+      <c r="G7" s="50"/>
+      <c r="H7" s="51"/>
     </row>
     <row r="8" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
@@ -1232,16 +1238,16 @@
       </c>
     </row>
     <row r="16" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="43" t="s">
+      <c r="A16" s="49" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="44"/>
-      <c r="C16" s="44"/>
-      <c r="D16" s="44"/>
-      <c r="E16" s="44"/>
-      <c r="F16" s="44"/>
-      <c r="G16" s="44"/>
-      <c r="H16" s="45"/>
+      <c r="B16" s="50"/>
+      <c r="C16" s="50"/>
+      <c r="D16" s="50"/>
+      <c r="E16" s="50"/>
+      <c r="F16" s="50"/>
+      <c r="G16" s="50"/>
+      <c r="H16" s="51"/>
     </row>
     <row r="17" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="22" t="s">
@@ -1357,13 +1363,13 @@
     </row>
     <row r="23" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="12"/>
-      <c r="B23" s="46" t="s">
+      <c r="B23" s="56" t="s">
         <v>18</v>
       </c>
-      <c r="C23" s="42"/>
-      <c r="D23" s="42"/>
-      <c r="E23" s="42"/>
-      <c r="F23" s="42"/>
+      <c r="C23" s="55"/>
+      <c r="D23" s="55"/>
+      <c r="E23" s="55"/>
+      <c r="F23" s="55"/>
       <c r="G23" s="15">
         <f>SUM(G18:G22)</f>
         <v>1250</v>
@@ -1374,13 +1380,13 @@
     </row>
     <row r="24" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="12"/>
-      <c r="B24" s="46" t="s">
+      <c r="B24" s="56" t="s">
         <v>19</v>
       </c>
-      <c r="C24" s="42"/>
-      <c r="D24" s="42"/>
-      <c r="E24" s="42"/>
-      <c r="F24" s="42"/>
+      <c r="C24" s="55"/>
+      <c r="D24" s="55"/>
+      <c r="E24" s="55"/>
+      <c r="F24" s="55"/>
       <c r="G24" s="23">
         <v>0.25</v>
       </c>
@@ -1388,13 +1394,13 @@
     </row>
     <row r="25" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="24"/>
-      <c r="B25" s="47" t="s">
+      <c r="B25" s="57" t="s">
         <v>20</v>
       </c>
-      <c r="C25" s="42"/>
-      <c r="D25" s="42"/>
-      <c r="E25" s="42"/>
-      <c r="F25" s="42"/>
+      <c r="C25" s="55"/>
+      <c r="D25" s="55"/>
+      <c r="E25" s="55"/>
+      <c r="F25" s="55"/>
       <c r="G25" s="15">
         <f>G23*(1+G24)</f>
         <v>1562.5</v>
@@ -1442,13 +1448,13 @@
     </row>
     <row r="28" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="29"/>
-      <c r="B28" s="48" t="s">
+      <c r="B28" s="58" t="s">
         <v>25</v>
       </c>
-      <c r="C28" s="49"/>
-      <c r="D28" s="49"/>
-      <c r="E28" s="49"/>
-      <c r="F28" s="49"/>
+      <c r="C28" s="47"/>
+      <c r="D28" s="47"/>
+      <c r="E28" s="47"/>
+      <c r="F28" s="47"/>
       <c r="G28" s="28">
         <f>G27-G25</f>
         <v>-562.5</v>
@@ -1498,11 +1504,11 @@
         <v>3</v>
       </c>
       <c r="F30">
-        <v>567</v>
+        <v>560</v>
       </c>
       <c r="G30" s="15">
         <f t="shared" ref="G30" si="3">E30*F30</f>
-        <v>1701</v>
+        <v>1680</v>
       </c>
       <c r="H30" s="16" t="s">
         <v>14</v>
@@ -1510,11 +1516,24 @@
     </row>
     <row r="31" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="12"/>
-      <c r="D31" s="14"/>
-      <c r="E31" s="14"/>
+      <c r="B31" t="s">
+        <v>56</v>
+      </c>
+      <c r="C31">
+        <v>4326</v>
+      </c>
+      <c r="D31" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="E31" s="14">
+        <v>1</v>
+      </c>
+      <c r="F31">
+        <v>300</v>
+      </c>
       <c r="G31" s="15">
         <f t="shared" ref="G31:G33" si="4">E31*F31</f>
-        <v>0</v>
+        <v>300</v>
       </c>
       <c r="H31" s="16" t="s">
         <v>14</v>
@@ -1546,16 +1565,16 @@
     </row>
     <row r="34" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="12"/>
-      <c r="B34" s="46" t="s">
+      <c r="B34" s="56" t="s">
         <v>18</v>
       </c>
-      <c r="C34" s="42"/>
-      <c r="D34" s="42"/>
-      <c r="E34" s="42"/>
-      <c r="F34" s="42"/>
+      <c r="C34" s="55"/>
+      <c r="D34" s="55"/>
+      <c r="E34" s="55"/>
+      <c r="F34" s="55"/>
       <c r="G34" s="15">
         <f>SUM(G30:G33)</f>
-        <v>1701</v>
+        <v>1980</v>
       </c>
       <c r="H34" s="16" t="s">
         <v>14</v>
@@ -1563,13 +1582,13 @@
     </row>
     <row r="35" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="12"/>
-      <c r="B35" s="46" t="s">
+      <c r="B35" s="56" t="s">
         <v>19</v>
       </c>
-      <c r="C35" s="42"/>
-      <c r="D35" s="42"/>
-      <c r="E35" s="42"/>
-      <c r="F35" s="42"/>
+      <c r="C35" s="55"/>
+      <c r="D35" s="55"/>
+      <c r="E35" s="55"/>
+      <c r="F35" s="55"/>
       <c r="G35" s="23">
         <v>0.25</v>
       </c>
@@ -1577,16 +1596,16 @@
     </row>
     <row r="36" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="24"/>
-      <c r="B36" s="47" t="s">
+      <c r="B36" s="57" t="s">
         <v>27</v>
       </c>
-      <c r="C36" s="42"/>
-      <c r="D36" s="42"/>
-      <c r="E36" s="42"/>
-      <c r="F36" s="42"/>
+      <c r="C36" s="55"/>
+      <c r="D36" s="55"/>
+      <c r="E36" s="55"/>
+      <c r="F36" s="55"/>
       <c r="G36" s="15">
         <f>G34*(1+G35)</f>
-        <v>2126.25</v>
+        <v>2475</v>
       </c>
       <c r="H36" s="16" t="s">
         <v>14</v>
@@ -1619,11 +1638,11 @@
         <v>1</v>
       </c>
       <c r="F38" s="27">
-        <v>1000</v>
+        <v>2500</v>
       </c>
       <c r="G38" s="28">
         <f>E38*F38</f>
-        <v>1000</v>
+        <v>2500</v>
       </c>
       <c r="H38" s="16" t="s">
         <v>14</v>
@@ -1631,16 +1650,16 @@
     </row>
     <row r="39" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="29"/>
-      <c r="B39" s="48" t="s">
+      <c r="B39" s="58" t="s">
         <v>29</v>
       </c>
-      <c r="C39" s="49"/>
-      <c r="D39" s="49"/>
-      <c r="E39" s="49"/>
-      <c r="F39" s="49"/>
+      <c r="C39" s="47"/>
+      <c r="D39" s="47"/>
+      <c r="E39" s="47"/>
+      <c r="F39" s="47"/>
       <c r="G39" s="28">
         <f>G38-G36</f>
-        <v>-1126.25</v>
+        <v>25</v>
       </c>
       <c r="H39" s="16" t="s">
         <v>14</v>
@@ -1699,11 +1718,24 @@
     </row>
     <row r="42" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="12"/>
-      <c r="D42" s="14"/>
-      <c r="E42" s="14"/>
+      <c r="B42" t="s">
+        <v>56</v>
+      </c>
+      <c r="C42">
+        <v>4326</v>
+      </c>
+      <c r="D42" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="E42" s="14">
+        <v>1</v>
+      </c>
+      <c r="F42">
+        <v>300</v>
+      </c>
       <c r="G42" s="15">
         <f t="shared" ref="G42:G44" si="6">E42*F42</f>
-        <v>0</v>
+        <v>300</v>
       </c>
       <c r="H42" s="16" t="s">
         <v>14</v>
@@ -1735,16 +1767,16 @@
     </row>
     <row r="45" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="12"/>
-      <c r="B45" s="46" t="s">
+      <c r="B45" s="56" t="s">
         <v>18</v>
       </c>
-      <c r="C45" s="42"/>
-      <c r="D45" s="42"/>
-      <c r="E45" s="42"/>
-      <c r="F45" s="42"/>
+      <c r="C45" s="55"/>
+      <c r="D45" s="55"/>
+      <c r="E45" s="55"/>
+      <c r="F45" s="55"/>
       <c r="G45" s="15">
         <f>SUM(G40:G44)</f>
-        <v>1000</v>
+        <v>1300</v>
       </c>
       <c r="H45" s="16" t="s">
         <v>14</v>
@@ -1752,13 +1784,13 @@
     </row>
     <row r="46" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="12"/>
-      <c r="B46" s="46" t="s">
+      <c r="B46" s="56" t="s">
         <v>19</v>
       </c>
-      <c r="C46" s="42"/>
-      <c r="D46" s="42"/>
-      <c r="E46" s="42"/>
-      <c r="F46" s="42"/>
+      <c r="C46" s="55"/>
+      <c r="D46" s="55"/>
+      <c r="E46" s="55"/>
+      <c r="F46" s="55"/>
       <c r="G46" s="23">
         <v>0.25</v>
       </c>
@@ -1766,16 +1798,16 @@
     </row>
     <row r="47" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="12"/>
-      <c r="B47" s="47" t="s">
+      <c r="B47" s="57" t="s">
         <v>31</v>
       </c>
-      <c r="C47" s="42"/>
-      <c r="D47" s="42"/>
-      <c r="E47" s="42"/>
-      <c r="F47" s="42"/>
+      <c r="C47" s="55"/>
+      <c r="D47" s="55"/>
+      <c r="E47" s="55"/>
+      <c r="F47" s="55"/>
       <c r="G47" s="15">
         <f>G45*(1+G46)</f>
-        <v>1250</v>
+        <v>1625</v>
       </c>
       <c r="H47" s="16" t="s">
         <v>14</v>
@@ -1806,11 +1838,11 @@
         <v>1</v>
       </c>
       <c r="F49">
-        <v>250</v>
+        <v>2000</v>
       </c>
       <c r="G49" s="15">
         <f t="shared" ref="G49" si="7">E49*F49</f>
-        <v>250</v>
+        <v>2000</v>
       </c>
       <c r="H49" s="16" t="s">
         <v>14</v>
@@ -1818,16 +1850,16 @@
     </row>
     <row r="50" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="12"/>
-      <c r="B50" s="50" t="s">
+      <c r="B50" s="54" t="s">
         <v>33</v>
       </c>
-      <c r="C50" s="42"/>
-      <c r="D50" s="42"/>
-      <c r="E50" s="42"/>
-      <c r="F50" s="42"/>
+      <c r="C50" s="55"/>
+      <c r="D50" s="55"/>
+      <c r="E50" s="55"/>
+      <c r="F50" s="55"/>
       <c r="G50" s="28">
         <f>G49-G47</f>
-        <v>-1000</v>
+        <v>375</v>
       </c>
       <c r="H50" s="16" t="s">
         <v>14</v>
@@ -1844,38 +1876,38 @@
       <c r="H51" s="34"/>
     </row>
     <row r="52" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="43" t="s">
+      <c r="A52" s="49" t="s">
         <v>34</v>
       </c>
-      <c r="B52" s="44"/>
-      <c r="C52" s="44"/>
-      <c r="D52" s="44"/>
-      <c r="E52" s="44"/>
-      <c r="F52" s="44"/>
-      <c r="G52" s="44"/>
-      <c r="H52" s="45"/>
+      <c r="B52" s="50"/>
+      <c r="C52" s="50"/>
+      <c r="D52" s="50"/>
+      <c r="E52" s="50"/>
+      <c r="F52" s="50"/>
+      <c r="G52" s="50"/>
+      <c r="H52" s="51"/>
     </row>
     <row r="53" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="51"/>
-      <c r="B53" s="49"/>
-      <c r="C53" s="49"/>
-      <c r="D53" s="49"/>
-      <c r="E53" s="49"/>
-      <c r="F53" s="49"/>
-      <c r="G53" s="49"/>
-      <c r="H53" s="52"/>
+      <c r="A53" s="46"/>
+      <c r="B53" s="47"/>
+      <c r="C53" s="47"/>
+      <c r="D53" s="47"/>
+      <c r="E53" s="47"/>
+      <c r="F53" s="47"/>
+      <c r="G53" s="47"/>
+      <c r="H53" s="48"/>
     </row>
     <row r="54" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="43" t="s">
+      <c r="A54" s="49" t="s">
         <v>35</v>
       </c>
-      <c r="B54" s="44"/>
-      <c r="C54" s="44"/>
-      <c r="D54" s="44"/>
-      <c r="E54" s="44"/>
-      <c r="F54" s="44"/>
-      <c r="G54" s="44"/>
-      <c r="H54" s="45"/>
+      <c r="B54" s="50"/>
+      <c r="C54" s="50"/>
+      <c r="D54" s="50"/>
+      <c r="E54" s="50"/>
+      <c r="F54" s="50"/>
+      <c r="G54" s="50"/>
+      <c r="H54" s="51"/>
     </row>
     <row r="55" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="22" t="s">
@@ -1940,7 +1972,7 @@
       <c r="H57" s="40"/>
     </row>
     <row r="58" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="53" t="s">
+      <c r="A58" s="52" t="s">
         <v>42</v>
       </c>
       <c r="B58" s="26" t="s">
@@ -1967,7 +1999,7 @@
       </c>
     </row>
     <row r="59" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="54"/>
+      <c r="A59" s="53"/>
       <c r="B59" s="17" t="s">
         <v>15</v>
       </c>
@@ -1992,7 +2024,7 @@
       </c>
     </row>
     <row r="60" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="54"/>
+      <c r="A60" s="53"/>
       <c r="B60" t="s">
         <v>48</v>
       </c>
@@ -2018,13 +2050,13 @@
     </row>
     <row r="61" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="39"/>
-      <c r="B61" s="50" t="s">
+      <c r="B61" s="54" t="s">
         <v>43</v>
       </c>
-      <c r="C61" s="42"/>
-      <c r="D61" s="42"/>
-      <c r="E61" s="42"/>
-      <c r="F61" s="42"/>
+      <c r="C61" s="55"/>
+      <c r="D61" s="55"/>
+      <c r="E61" s="55"/>
+      <c r="F61" s="55"/>
       <c r="G61" s="37">
         <f>G56-SUM(G58:G60)</f>
         <v>2750</v>
@@ -2034,17 +2066,28 @@
       </c>
     </row>
     <row r="62" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="55"/>
-      <c r="B62" s="56"/>
-      <c r="C62" s="56"/>
-      <c r="D62" s="57"/>
-      <c r="E62" s="57"/>
-      <c r="F62" s="57"/>
-      <c r="G62" s="58"/>
-      <c r="H62" s="59"/>
+      <c r="A62" s="41"/>
+      <c r="B62" s="42"/>
+      <c r="C62" s="42"/>
+      <c r="D62" s="43"/>
+      <c r="E62" s="43"/>
+      <c r="F62" s="43"/>
+      <c r="G62" s="44"/>
+      <c r="H62" s="45"/>
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A7:H7"/>
+    <mergeCell ref="A16:H16"/>
+    <mergeCell ref="B23:F23"/>
+    <mergeCell ref="B24:F24"/>
+    <mergeCell ref="B39:F39"/>
+    <mergeCell ref="B25:F25"/>
+    <mergeCell ref="B28:F28"/>
+    <mergeCell ref="B34:F34"/>
+    <mergeCell ref="B35:F35"/>
+    <mergeCell ref="B36:F36"/>
     <mergeCell ref="A53:H53"/>
     <mergeCell ref="A54:H54"/>
     <mergeCell ref="A58:A60"/>
@@ -2054,17 +2097,6 @@
     <mergeCell ref="B47:F47"/>
     <mergeCell ref="B50:F50"/>
     <mergeCell ref="A52:H52"/>
-    <mergeCell ref="B39:F39"/>
-    <mergeCell ref="B25:F25"/>
-    <mergeCell ref="B28:F28"/>
-    <mergeCell ref="B34:F34"/>
-    <mergeCell ref="B35:F35"/>
-    <mergeCell ref="B36:F36"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="A7:H7"/>
-    <mergeCell ref="A16:H16"/>
-    <mergeCell ref="B23:F23"/>
-    <mergeCell ref="B24:F24"/>
   </mergeCells>
   <conditionalFormatting sqref="G28 G39 G50">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">

</xml_diff>